<commit_message>
producto y balance general
</commit_message>
<xml_diff>
--- a/example_reports/EJEMPLO-DATOS-PRODUCTOS.xlsx
+++ b/example_reports/EJEMPLO-DATOS-PRODUCTOS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Esteban Suarez Prado\Agil\example_reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\agil_\example_reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="26">
   <si>
     <t>Codigo</t>
   </si>
@@ -87,6 +87,18 @@
   </si>
   <si>
     <t>texto marca</t>
+  </si>
+  <si>
+    <t>Tipo Producto</t>
+  </si>
+  <si>
+    <t>base</t>
+  </si>
+  <si>
+    <t>intermedio</t>
+  </si>
+  <si>
+    <t>final</t>
   </si>
 </sst>
 </file>
@@ -130,9 +142,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -437,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P15"/>
+  <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,7 +464,7 @@
     <col min="15" max="15" width="22.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -500,8 +513,11 @@
       <c r="P1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -550,8 +566,11 @@
       <c r="P2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -600,8 +619,11 @@
       <c r="P3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -650,8 +672,11 @@
       <c r="P4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -700,8 +725,11 @@
       <c r="P5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -750,8 +778,11 @@
       <c r="P6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -800,8 +831,11 @@
       <c r="P7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -850,8 +884,11 @@
       <c r="P8" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -900,8 +937,11 @@
       <c r="P9" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -950,8 +990,11 @@
       <c r="P10" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1000,8 +1043,11 @@
       <c r="P11" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1050,8 +1096,11 @@
       <c r="P12" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1100,8 +1149,11 @@
       <c r="P13" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1150,8 +1202,11 @@
       <c r="P14" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1200,10 +1255,16 @@
       <c r="P15" t="s">
         <v>21</v>
       </c>
+      <c r="Q15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O17" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
reportes y algunos cambios
</commit_message>
<xml_diff>
--- a/example_reports/EJEMPLO-DATOS-PRODUCTOS.xlsx
+++ b/example_reports/EJEMPLO-DATOS-PRODUCTOS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\agil_\example_reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Esteban Suarez Prado\Agil\example_reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="27">
   <si>
     <t>Codigo</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>final</t>
+  </si>
+  <si>
+    <t>toto</t>
   </si>
 </sst>
 </file>
@@ -453,7 +456,7 @@
   <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+      <selection activeCell="G2" sqref="G2:G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,8 +539,8 @@
       <c r="F2">
         <v>3</v>
       </c>
-      <c r="G2">
-        <v>123</v>
+      <c r="G2" t="s">
+        <v>26</v>
       </c>
       <c r="H2">
         <v>12</v>
@@ -589,8 +592,8 @@
       <c r="F3">
         <v>3</v>
       </c>
-      <c r="G3">
-        <v>123</v>
+      <c r="G3" t="s">
+        <v>26</v>
       </c>
       <c r="H3">
         <v>12</v>
@@ -642,8 +645,8 @@
       <c r="F4">
         <v>3</v>
       </c>
-      <c r="G4">
-        <v>123</v>
+      <c r="G4" t="s">
+        <v>26</v>
       </c>
       <c r="H4">
         <v>12</v>
@@ -695,8 +698,8 @@
       <c r="F5">
         <v>3</v>
       </c>
-      <c r="G5">
-        <v>123</v>
+      <c r="G5" t="s">
+        <v>26</v>
       </c>
       <c r="H5">
         <v>12</v>
@@ -748,8 +751,8 @@
       <c r="F6">
         <v>3</v>
       </c>
-      <c r="G6">
-        <v>123</v>
+      <c r="G6" t="s">
+        <v>26</v>
       </c>
       <c r="H6">
         <v>12</v>
@@ -801,8 +804,8 @@
       <c r="F7">
         <v>3</v>
       </c>
-      <c r="G7">
-        <v>123</v>
+      <c r="G7" t="s">
+        <v>26</v>
       </c>
       <c r="H7">
         <v>12</v>
@@ -854,8 +857,8 @@
       <c r="F8">
         <v>3</v>
       </c>
-      <c r="G8">
-        <v>123</v>
+      <c r="G8" t="s">
+        <v>26</v>
       </c>
       <c r="H8">
         <v>12</v>
@@ -907,8 +910,8 @@
       <c r="F9">
         <v>3</v>
       </c>
-      <c r="G9">
-        <v>123</v>
+      <c r="G9" t="s">
+        <v>26</v>
       </c>
       <c r="H9">
         <v>12</v>
@@ -960,8 +963,8 @@
       <c r="F10">
         <v>3</v>
       </c>
-      <c r="G10">
-        <v>123</v>
+      <c r="G10" t="s">
+        <v>26</v>
       </c>
       <c r="H10">
         <v>12</v>
@@ -1013,8 +1016,8 @@
       <c r="F11">
         <v>3</v>
       </c>
-      <c r="G11">
-        <v>123</v>
+      <c r="G11" t="s">
+        <v>26</v>
       </c>
       <c r="H11">
         <v>12</v>
@@ -1066,8 +1069,8 @@
       <c r="F12">
         <v>3</v>
       </c>
-      <c r="G12">
-        <v>123</v>
+      <c r="G12" t="s">
+        <v>26</v>
       </c>
       <c r="H12">
         <v>12</v>
@@ -1119,8 +1122,8 @@
       <c r="F13">
         <v>3</v>
       </c>
-      <c r="G13">
-        <v>123</v>
+      <c r="G13" t="s">
+        <v>26</v>
       </c>
       <c r="H13">
         <v>12</v>
@@ -1172,8 +1175,8 @@
       <c r="F14">
         <v>3</v>
       </c>
-      <c r="G14">
-        <v>123</v>
+      <c r="G14" t="s">
+        <v>26</v>
       </c>
       <c r="H14">
         <v>12</v>
@@ -1225,8 +1228,8 @@
       <c r="F15">
         <v>3</v>
       </c>
-      <c r="G15">
-        <v>123</v>
+      <c r="G15" t="s">
+        <v>26</v>
       </c>
       <c r="H15">
         <v>12</v>

</xml_diff>